<commit_message>
first implementation of Car and movement
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="entry_params" sheetId="3" r:id="rId2"/>
     <sheet name="scheme" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -663,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F2">
         <v>60</v>
@@ -674,13 +674,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="F3">
         <v>60</v>
@@ -688,16 +688,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="F4">
         <v>60</v>
@@ -708,16 +708,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="F5">
         <v>60</v>
@@ -728,16 +728,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="F6">
         <v>60</v>
@@ -748,16 +748,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F7">
         <v>60</v>
@@ -768,16 +768,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="F8">
         <v>60</v>
@@ -788,16 +788,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="F9">
         <v>60</v>
@@ -808,16 +808,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="F10">
         <v>60</v>
@@ -828,16 +828,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="F11">
         <v>60</v>
@@ -851,13 +851,13 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="D12">
-        <v>-1</v>
+        <v>-100</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="F12">
         <v>60</v>
@@ -868,16 +868,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>-1</v>
+        <v>-100</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="D13">
-        <v>-2</v>
+        <v>-200</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="F13">
         <v>60</v>
@@ -888,16 +888,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>-2</v>
+        <v>-200</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="D14">
-        <v>-3</v>
+        <v>-300</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="F14">
         <v>60</v>
@@ -911,13 +911,13 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="F15">
         <v>60</v>
@@ -931,13 +931,13 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="F16">
         <v>60</v>
@@ -948,16 +948,16 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17">
-        <v>-1</v>
+        <v>-100</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="D17">
-        <v>-2</v>
+        <v>-200</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="F17">
         <v>60</v>
@@ -968,16 +968,16 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18">
-        <v>-2</v>
+        <v>-200</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="D18">
-        <v>-3</v>
+        <v>-300</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="F18">
         <v>60</v>
@@ -996,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1128,7 +1128,7 @@
   <dimension ref="A1:AX55"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added JavaFX app componet for visual rendering added movement wroking functionlity
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -621,7 +621,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,7 +683,7 @@
         <v>200</v>
       </c>
       <c r="F3">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -800,7 +800,7 @@
         <v>300</v>
       </c>
       <c r="F9">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -840,7 +840,7 @@
         <v>400</v>
       </c>
       <c r="F11">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
@@ -997,7 +997,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1031,7 +1031,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>0.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1045,7 +1045,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1059,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>0.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1073,7 +1073,7 @@
         <v>9</v>
       </c>
       <c r="D5">
-        <v>0.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1087,7 +1087,7 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1128,7 +1128,7 @@
   <dimension ref="A1:AX55"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
implemented dynamic scaling on UI
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -620,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1031,7 +1031,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1045,7 +1045,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1059,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1073,7 +1073,7 @@
         <v>9</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1087,7 +1087,7 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1101,7 +1101,7 @@
         <v>11</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1115,7 +1115,7 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>